<commit_message>
adding config for kpis
</commit_message>
<xml_diff>
--- a/Projects/CARLSBRGHK/Data/KPI_Assortment_Template.xlsx
+++ b/Projects/CARLSBRGHK/Data/KPI_Assortment_Template.xlsx
@@ -68,10 +68,10 @@
     <t xml:space="preserve">DIS_Ambient</t>
   </si>
   <si>
-    <t xml:space="preserve">country</t>
+    <t xml:space="preserve">is_active</t>
   </si>
   <si>
-    <t xml:space="preserve">Hong kong</t>
+    <t xml:space="preserve">Y</t>
   </si>
   <si>
     <t xml:space="preserve">DIS_Cooler</t>
@@ -215,7 +215,7 @@
     <numFmt numFmtId="165" formatCode="0"/>
     <numFmt numFmtId="166" formatCode="MM/DD/YYYY"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -253,12 +253,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="5">
@@ -387,7 +381,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="28">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -496,10 +490,6 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -597,9 +587,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>2582640</xdr:colOff>
+      <xdr:colOff>2582280</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>402480</xdr:rowOff>
+      <xdr:rowOff>402120</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -613,7 +603,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="1705680" y="77040"/>
-          <a:ext cx="876960" cy="325440"/>
+          <a:ext cx="876600" cy="325080"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -681,9 +671,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>813240</xdr:colOff>
+      <xdr:colOff>812880</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>9000</xdr:rowOff>
+      <xdr:rowOff>8640</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -697,7 +687,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="294120" y="0"/>
-          <a:ext cx="519120" cy="513720"/>
+          <a:ext cx="518760" cy="513360"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -723,9 +713,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>973440</xdr:colOff>
+      <xdr:colOff>973080</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>401040</xdr:rowOff>
+      <xdr:rowOff>400680</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -738,8 +728,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1808280" y="86760"/>
-          <a:ext cx="907920" cy="314280"/>
+          <a:off x="1818000" y="86760"/>
+          <a:ext cx="907560" cy="313920"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -807,9 +797,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>1068480</xdr:colOff>
+      <xdr:colOff>1068120</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>9000</xdr:rowOff>
+      <xdr:rowOff>8640</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -823,7 +813,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="549360" y="0"/>
-          <a:ext cx="519120" cy="513720"/>
+          <a:ext cx="518760" cy="513360"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -867,22 +857,22 @@
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="B19" activeCellId="0" sqref="B19"/>
+      <selection pane="bottomLeft" activeCell="A20" activeCellId="0" sqref="A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="43.3846153846154"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="22.6032388663968"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="20.246963562753"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="22.6032388663968"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="34.8137651821862"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="22.9230769230769"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="20.246963562753"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="20.4615384615385"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="23.8866396761134"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="24.1012145748988"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="23.8866396761134"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="43.7044534412956"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="22.7085020242915"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="20.3522267206478"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="22.7085020242915"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="35.0283400809717"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="23.0323886639676"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="20.3522267206478"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="20.5668016194332"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="24.1012145748988"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="24.3157894736842"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="24.1012145748988"/>
     <col collapsed="false" hidden="false" max="1025" min="12" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -1021,9 +1011,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="9" width="19.6032388663968"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="9" width="27.4210526315789"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="10" width="17.3522267206478"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="9" width="19.7085020242915"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="9" width="27.6356275303644"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="10" width="17.4615384615385"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="11" width="10.3886639676113"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="11" width="8.24696356275304"/>
     <col collapsed="false" hidden="false" max="181" min="6" style="9" width="9.10526315789474"/>
@@ -5180,7 +5170,7 @@
       <c r="A6" s="21" t="s">
         <v>14</v>
       </c>
-      <c r="B6" s="27" t="s">
+      <c r="B6" s="21" t="s">
         <v>20</v>
       </c>
       <c r="C6" s="22" t="s">
@@ -8282,7 +8272,7 @@
       <c r="A9" s="21" t="s">
         <v>14</v>
       </c>
-      <c r="B9" s="27" t="s">
+      <c r="B9" s="21" t="s">
         <v>20</v>
       </c>
       <c r="C9" s="22" t="s">
@@ -35337,13 +35327,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="9" width="88.4817813765182"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="9" width="67.5910931174089"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="9" width="89.2307692307692"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="9" width="68.1295546558705"/>
     <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="9.10526315789474"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="28" t="s">
+      <c r="A1" s="27" t="s">
         <v>49</v>
       </c>
       <c r="B1" s="0"/>

</xml_diff>